<commit_message>
- Diagramas de clases y casos de usos del PFC
</commit_message>
<xml_diff>
--- a/MemoriaPFC/PlanificacionPFC.xlsx
+++ b/MemoriaPFC/PlanificacionPFC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="21315" windowHeight="10035"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="19320" windowHeight="10035"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -81,9 +81,6 @@
     <t>Patron Agente Singleton. Tabla de propuestas autorreferenciada, como en el patron composite</t>
   </si>
   <si>
-    <t>Fabricaciones puras; Gestor de base de datos que puede acceder a varias bases de datos, sincronizando los cambios (patrón Observador)</t>
-  </si>
-  <si>
     <t>Comenzada la implementación del TreeViewer y de la perspectiva</t>
   </si>
   <si>
@@ -103,6 +100,9 @@
   </si>
   <si>
     <t>Analisis</t>
+  </si>
+  <si>
+    <t>Fabricaciones puras; Gestor de base de datos que puede acceder a varias bases de datos, sincronizando los cambios (patrón Observador). Patron Command</t>
   </si>
 </sst>
 </file>
@@ -489,8 +489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,7 +511,7 @@
         <v>3</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -526,7 +526,7 @@
       </c>
       <c r="H3" s="10"/>
       <c r="I3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -541,7 +541,7 @@
       </c>
       <c r="H4" s="7"/>
       <c r="I4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -553,7 +553,7 @@
       </c>
       <c r="H5" s="9"/>
       <c r="I5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -607,7 +607,7 @@
         <v>40491</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>12</v>
@@ -632,7 +632,7 @@
         <v>18</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -640,7 +640,7 @@
         <v>40501</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -648,7 +648,7 @@
         <v>40502</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>